<commit_message>
updated html, minor comments for app.py
</commit_message>
<xml_diff>
--- a/Resources/annual_home_sales.xlsx
+++ b/Resources/annual_home_sales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab74b0f1fe3ad570/Desktop/Challenges/Austin_Housing_Market/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{8D16774B-6510-4E17-975F-1AB71A26F248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BB89775-0123-463E-ACF7-EDFDA96A05FA}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{8D16774B-6510-4E17-975F-1AB71A26F248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{535FE581-A69A-4631-B376-7A5F6B37938A}"/>
   <bookViews>
-    <workbookView xWindow="6036" yWindow="2676" windowWidth="23040" windowHeight="12204" xr2:uid="{8E51AF81-628F-4BD7-98C2-07564C4485AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{8E51AF81-628F-4BD7-98C2-07564C4485AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,6 +167,3202 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>median_price</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$34</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>72252</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75865</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82929</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90949</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95158</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>107884</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>111819</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>117207</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>125888</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>143550</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>149611</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>153545</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>153836</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>153198</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160701</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>171272</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>183292</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>187319</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>185150</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>189356</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>189000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>202500</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>220000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>239900</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>260000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>280000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>295000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>305000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>315000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>344990</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>451500</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>501506</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C65D-4DDC-A880-9B8F99782146}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1323518511"/>
+        <c:axId val="1323519471"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1323518511"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1323519471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1323519471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1323518511"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total_listings</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$34</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>4412</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3552</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2860</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3645</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3778</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5126</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5344</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4318</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3292</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8163</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9669</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9723</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8297</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8028</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9163</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10911</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10131</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10906</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9066</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7021</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5441</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5651</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5806</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6237</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7129</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7288</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6887</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4490</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2307</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1FC4-470B-BBC9-A97DB02FE39F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1324575119"/>
+        <c:axId val="1324573679"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1324575119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1324573679"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1324573679"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1324575119"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>7068</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7485</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8389</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9784</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10418</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11291</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12406</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12253</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15338</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17845</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18321</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18095</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18414</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19469</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22193</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26448</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29767</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27571</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22068</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20407</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19547</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20972</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>25131</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>29901</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>30054</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>31287</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>32488</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>33718</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>34581</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>37005</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>40197</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41079</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1536-409F-8F6D-2ED6DF3533FB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1627209359"/>
+        <c:axId val="1627074703"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1627209359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1627074703"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1627074703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1627209359"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0FA90CD-268D-5174-A5CC-5C7618A2D70B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DD21F50-9A0D-B988-F51F-47BC4FBB84AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>54429</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>385899</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>488769</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>181792</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50695A3B-5A80-DFBA-D372-0C69789F7928}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -466,13 +3662,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2698380B-2A6B-4ACD-9581-ABFF55C0294D}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AF23" sqref="AF23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33" thickBot="1" x14ac:dyDescent="0.45">
@@ -1259,5 +4459,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>